<commit_message>
Replace vat data with original from OECD
</commit_message>
<xml_diff>
--- a/source_data/vat-gst-rates-historical-tax-database.xlsx
+++ b/source_data/vat-gst-rates-historical-tax-database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\consumption-taxes\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2584BBF7-A6E2-4671-B46F-04E6CA5946A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D2B78D0-2CDC-44B5-BDBF-9053F90002D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="16080" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3211" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3212" uniqueCount="234">
   <si>
     <t>Australia</t>
   </si>
@@ -423,6 +423,9 @@
     </r>
   </si>
   <si>
+    <t>Reduced rate</t>
+  </si>
+  <si>
     <t>1.0/3.0/6.0/9.0</t>
   </si>
   <si>
@@ -476,6 +479,12 @@
   </si>
   <si>
     <t>4.0/9.0/12</t>
+  </si>
+  <si>
+    <t>4.0/9.012.0</t>
+  </si>
+  <si>
+    <t>4.0/9.013.0</t>
   </si>
   <si>
     <t>4.0/10.0/16.0</t>
@@ -860,6 +869,9 @@
     <t>Lithuania</t>
   </si>
   <si>
+    <t>19.0 - 21.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.0/9.0 </t>
   </si>
   <si>
@@ -941,12 +953,6 @@
   </si>
   <si>
     <t>5.0/9.5</t>
-  </si>
-  <si>
-    <t>4.0/9.0/13.0</t>
-  </si>
-  <si>
-    <t>4.0/9.0/12.0</t>
   </si>
 </sst>
 </file>
@@ -1386,9 +1392,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1397,6 +1400,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1748,10 +1754,10 @@
   <dimension ref="A1:BL283"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="S117" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y124" sqref="Y124"/>
+      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1814,54 +1820,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" x14ac:dyDescent="0.2">
-      <c r="B1" s="121" t="s">
-        <v>144</v>
-      </c>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="121"/>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
-      <c r="P1" s="121"/>
-      <c r="Q1" s="121"/>
-      <c r="R1" s="121"/>
-      <c r="S1" s="121"/>
-      <c r="T1" s="121"/>
-      <c r="U1" s="121"/>
-      <c r="V1" s="121"/>
-      <c r="W1" s="121"/>
-      <c r="X1" s="121"/>
-      <c r="Y1" s="121"/>
-      <c r="Z1" s="121"/>
-      <c r="AA1" s="121"/>
-      <c r="AB1" s="121"/>
-      <c r="AC1" s="121"/>
-      <c r="AD1" s="121"/>
-      <c r="AE1" s="121"/>
-      <c r="AF1" s="121"/>
-      <c r="AG1" s="121"/>
-      <c r="AH1" s="121"/>
-      <c r="AI1" s="121"/>
-      <c r="AJ1" s="121"/>
-      <c r="AK1" s="121"/>
-      <c r="AL1" s="121"/>
-      <c r="AM1" s="121"/>
-      <c r="AN1" s="121"/>
-      <c r="AO1" s="121"/>
-      <c r="AP1" s="121"/>
-      <c r="AQ1" s="121"/>
-      <c r="AR1" s="121"/>
-      <c r="AS1" s="121"/>
-      <c r="AT1" s="121"/>
-      <c r="AU1" s="121"/>
+      <c r="B1" s="124" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124"/>
+      <c r="M1" s="124"/>
+      <c r="N1" s="124"/>
+      <c r="O1" s="124"/>
+      <c r="P1" s="124"/>
+      <c r="Q1" s="124"/>
+      <c r="R1" s="124"/>
+      <c r="S1" s="124"/>
+      <c r="T1" s="124"/>
+      <c r="U1" s="124"/>
+      <c r="V1" s="124"/>
+      <c r="W1" s="124"/>
+      <c r="X1" s="124"/>
+      <c r="Y1" s="124"/>
+      <c r="Z1" s="124"/>
+      <c r="AA1" s="124"/>
+      <c r="AB1" s="124"/>
+      <c r="AC1" s="124"/>
+      <c r="AD1" s="124"/>
+      <c r="AE1" s="124"/>
+      <c r="AF1" s="124"/>
+      <c r="AG1" s="124"/>
+      <c r="AH1" s="124"/>
+      <c r="AI1" s="124"/>
+      <c r="AJ1" s="124"/>
+      <c r="AK1" s="124"/>
+      <c r="AL1" s="124"/>
+      <c r="AM1" s="124"/>
+      <c r="AN1" s="124"/>
+      <c r="AO1" s="124"/>
+      <c r="AP1" s="124"/>
+      <c r="AQ1" s="124"/>
+      <c r="AR1" s="124"/>
+      <c r="AS1" s="124"/>
+      <c r="AT1" s="124"/>
+      <c r="AU1" s="124"/>
     </row>
     <row r="2" spans="1:64" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B2" s="7">
@@ -2907,82 +2913,82 @@
         <v>10</v>
       </c>
       <c r="AD11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AE11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AF11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AG11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AH11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AI11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AJ11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AK11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AL11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AM11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AN11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AO11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AP11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AQ11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AR11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AS11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AT11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AU11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AV11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AW11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AX11" s="52" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="AY11" s="52" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="AZ11" s="52" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="BA11" s="52" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="BB11" s="52" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="BC11" s="52" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:64" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -4715,7 +4721,7 @@
     </row>
     <row r="30" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="47" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="45"/>
@@ -5883,7 +5889,7 @@
     </row>
     <row r="41" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="61" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B41" s="25"/>
       <c r="C41" s="88"/>
@@ -6537,7 +6543,7 @@
     </row>
     <row r="48" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="46" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B48" s="46"/>
       <c r="C48" s="11"/>
@@ -6818,100 +6824,100 @@
       <c r="P51" s="21"/>
       <c r="Q51" s="21"/>
       <c r="R51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="S51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="T51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="U51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="V51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="W51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="X51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="Y51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="Z51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AA51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AB51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AC51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AD51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AE51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AF51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AG51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AH51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AI51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AJ51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AK51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AL51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AM51" s="59" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="AN51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AO51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AP51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AQ51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AR51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AS51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AT51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AU51" s="59" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AV51" s="59" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="AW51" s="59" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="AX51" s="59" t="s">
         <v>25</v>
@@ -7012,94 +7018,94 @@
       <c r="P53" s="21"/>
       <c r="Q53" s="21"/>
       <c r="R53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="S53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="T53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="U53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="V53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="W53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="X53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="Y53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="Z53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AA53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AB53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AC53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AD53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AE53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AF53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AG53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AH53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AI53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AJ53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AK53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AL53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AM53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AN53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AO53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AP53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AQ53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AR53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AS53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AT53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AU53" s="59" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AV53" s="21"/>
       <c r="AW53" s="21"/>
@@ -7604,22 +7610,22 @@
         <v>15</v>
       </c>
       <c r="AX58" s="52" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="AY58" s="52" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="AZ58" s="52" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="BA58" s="52" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="BB58" s="52" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="BC58" s="52" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="59" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8205,7 +8211,7 @@
     </row>
     <row r="65" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="46" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="11"/>
@@ -8619,40 +8625,40 @@
         <v>25</v>
       </c>
       <c r="AR68" s="54" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AS68" s="54" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AT68" s="54" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AU68" s="54" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AV68" s="54" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AW68" s="54" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AX68" s="54" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AY68" s="54" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AZ68" s="54" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="BA68" s="54" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="BB68" s="54" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="BC68" s="54" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -9088,85 +9094,85 @@
         <v>16</v>
       </c>
       <c r="AC73" s="52" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AD73" s="52" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="AE73" s="52" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="AF73" s="52" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="AG73" s="52" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AH73" s="52" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AI73" s="52" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AJ73" s="52" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AK73" s="52" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AL73" s="52" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AM73" s="52" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AN73" s="52" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AO73" s="52" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AP73" s="52" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AQ73" s="52" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="AR73" s="52" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AS73" s="52" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="AT73" s="52" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="AU73" s="52" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="AV73" s="52" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="AW73" s="52" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="AX73" s="52" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="AY73" s="52" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="AZ73" s="52" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="BA73" s="52" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="BB73" s="52" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="BC73" s="52" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="74" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -9664,25 +9670,25 @@
         <v>46</v>
       </c>
       <c r="AW78" s="52" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="AX78" s="52" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="AY78" s="52" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="AZ78" s="52" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="BA78" s="52" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="BB78" s="52" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="BC78" s="52" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="79" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -10049,109 +10055,109 @@
       <c r="S83" s="108"/>
       <c r="T83" s="108"/>
       <c r="U83" s="108" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="V83" s="108" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="W83" s="108" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="X83" s="108" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="Y83" s="108" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="Z83" s="108" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="AA83" s="108" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="AB83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AC83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AD83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AE83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AF83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AG83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AH83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AI83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AJ83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AK83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AL83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AM83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AN83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AO83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AP83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AQ83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AR83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AS83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AT83" s="108" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AU83" s="109" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="AV83" s="109" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="AW83" s="109" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="AX83" s="109" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="AY83" s="109" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="AZ83" s="109" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="BA83" s="109" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="BB83" s="109" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="BC83" s="109" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="84" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -10219,7 +10225,7 @@
     </row>
     <row r="85" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="60" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B85" s="108"/>
       <c r="C85" s="108"/>
@@ -10255,67 +10261,67 @@
       <c r="AG85" s="108"/>
       <c r="AH85" s="108"/>
       <c r="AI85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AJ85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AK85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AL85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AM85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AN85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AO85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AP85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AQ85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AR85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AS85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AT85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AU85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AV85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AW85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AX85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AY85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AZ85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="BA85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="BB85" s="109" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="BC85" s="109" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="86" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -11725,7 +11731,7 @@
     </row>
     <row r="100" spans="1:55" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A100" s="98" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B100" s="25" t="s">
         <v>16</v>
@@ -12018,7 +12024,7 @@
       <c r="AV102" s="19"/>
       <c r="AW102" s="19"/>
       <c r="AX102" s="31" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="AY102" s="51">
         <v>42522</v>
@@ -12085,13 +12091,13 @@
         <v>16</v>
       </c>
       <c r="V103" s="52" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="W103" s="52" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="X103" s="52" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="Y103" s="52" t="s">
         <v>80</v>
@@ -12154,37 +12160,37 @@
         <v>80</v>
       </c>
       <c r="AS103" s="52" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="AT103" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AU103" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AV103" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AW103" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AX103" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AY103" s="52" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AZ103" s="52" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BA103" s="52" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BB103" s="52" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC103" s="52" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="104" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -12246,7 +12252,7 @@
       <c r="AV104" s="19"/>
       <c r="AW104" s="19"/>
       <c r="AX104" s="31" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="AY104" s="51">
         <v>42522</v>
@@ -13800,7 +13806,7 @@
         <v>92</v>
       </c>
       <c r="R120" s="59" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="S120" s="59" t="s">
         <v>94</v>
@@ -14531,7 +14537,7 @@
     </row>
     <row r="127" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="47" t="s">
-        <v>48</v>
+        <v>114</v>
       </c>
       <c r="B127" s="25" t="s">
         <v>16</v>
@@ -15077,67 +15083,67 @@
         <v>6</v>
       </c>
       <c r="K132" s="52" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="L132" s="52" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M132" s="52" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N132" s="52" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="O132" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="P132" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="P132" s="52" t="s">
-        <v>118</v>
-      </c>
       <c r="Q132" s="52" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="R132" s="52" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="S132" s="52" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="T132" s="52" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="U132" s="52" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="V132" s="52" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="W132" s="52" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="X132" s="52" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="Y132" s="52" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="Z132" s="52" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AA132" s="52" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AB132" s="52" t="s">
-        <v>231</v>
+        <v>128</v>
       </c>
       <c r="AC132" s="52" t="s">
-        <v>230</v>
+        <v>129</v>
       </c>
       <c r="AD132" s="52" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="AE132" s="52" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="AF132" s="52" t="s">
         <v>28</v>
@@ -15197,19 +15203,19 @@
         <v>28</v>
       </c>
       <c r="AY132" s="52" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AZ132" s="52" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BA132" s="52" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BB132" s="52" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="BC132" s="52" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="133" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -15321,31 +15327,31 @@
         <v>18</v>
       </c>
       <c r="J134" s="52" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K134" s="52" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L134" s="52" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M134" s="52" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N134" s="52" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="O134" s="52" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="P134" s="52" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Q134" s="52" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="R134" s="52" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="S134" s="54">
         <v>30</v>
@@ -15801,7 +15807,7 @@
     </row>
     <row r="139" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="47" t="s">
-        <v>48</v>
+        <v>114</v>
       </c>
       <c r="B139" s="25"/>
       <c r="C139" s="88"/>
@@ -16199,7 +16205,7 @@
     </row>
     <row r="144" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="47" t="s">
-        <v>48</v>
+        <v>114</v>
       </c>
       <c r="B144" s="25" t="s">
         <v>16</v>
@@ -16412,7 +16418,7 @@
     </row>
     <row r="146" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="46" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B146" s="10"/>
       <c r="C146" s="10"/>
@@ -16824,13 +16830,13 @@
         <v>12</v>
       </c>
       <c r="BA149" s="54" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="BB149" s="54" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="BC149" s="54" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="150" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -16880,7 +16886,7 @@
     </row>
     <row r="151" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="46" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B151" s="10"/>
       <c r="C151" s="10"/>
@@ -17053,8 +17059,8 @@
       <c r="AQ152" s="19">
         <v>18</v>
       </c>
-      <c r="AR152" s="19">
-        <v>19</v>
+      <c r="AR152" s="19" t="s">
+        <v>216</v>
       </c>
       <c r="AS152" s="21">
         <v>21</v>
@@ -17139,7 +17145,7 @@
       <c r="AP153" s="22"/>
       <c r="AQ153" s="21"/>
       <c r="AR153" s="53" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="AS153" s="21"/>
       <c r="AT153" s="53"/>
@@ -17242,64 +17248,64 @@
         <v>5</v>
       </c>
       <c r="AJ154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AK154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AL154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AM154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AN154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AO154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AP154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AQ154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AR154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AS154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AT154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AU154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AV154" s="52" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="AW154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AX154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AY154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AZ154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="BA154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="BB154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="BC154" s="52" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="155" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -17657,40 +17663,40 @@
         <v>4</v>
       </c>
       <c r="F159" s="52" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="G159" s="52" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H159" s="52" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="I159" s="52" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="J159" s="52" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="K159" s="52" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="L159" s="52" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="M159" s="52" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="N159" s="52" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="O159" s="52" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="P159" s="52" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="Q159" s="52" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="R159" s="52" t="s">
         <v>80</v>
@@ -17723,88 +17729,88 @@
         <v>80</v>
       </c>
       <c r="AB159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AC159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AD159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AE159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AF159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AG159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AI159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AJ159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AK159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AL159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AM159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AN159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AO159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AP159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AQ159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AR159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AS159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AT159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AU159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AV159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AW159" s="52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AX159" s="52" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="AY159" s="52" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="AZ159" s="52" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="BA159" s="52" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="BB159" s="52" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="BC159" s="52" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="160" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -18595,7 +18601,7 @@
     </row>
     <row r="168" spans="1:56" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A168" s="47" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B168" s="25" t="s">
         <v>16</v>
@@ -20048,25 +20054,25 @@
         <v>85</v>
       </c>
       <c r="AN181" s="52" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="AO181" s="52" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="AP181" s="52" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="AQ181" s="52" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="AR181" s="52" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="AS181" s="52" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="AT181" s="52" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="AU181" s="52" t="s">
         <v>47</v>
@@ -20081,19 +20087,19 @@
         <v>47</v>
       </c>
       <c r="AY181" s="52" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="AZ181" s="52" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="BA181" s="52" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="BB181" s="52" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="BC181" s="52" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="182" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -20554,37 +20560,37 @@
         <v>7</v>
       </c>
       <c r="AI186" s="89" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AJ186" s="89" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AK186" s="89" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AL186" s="89" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AM186" s="89" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AN186" s="89" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AO186" s="89" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AP186" s="89" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AQ186" s="89" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AR186" s="89" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AS186" s="89" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AT186" s="89" t="s">
         <v>34</v>
@@ -21035,22 +21041,22 @@
         <v>16</v>
       </c>
       <c r="U191" s="89" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="V191" s="89" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="W191" s="89" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="X191" s="89" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="Y191" s="89" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="Z191" s="89" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="AA191" s="41">
         <v>8</v>
@@ -21065,46 +21071,46 @@
         <v>5</v>
       </c>
       <c r="AE191" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AF191" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AG191" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AH191" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AI191" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AJ191" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AK191" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AL191" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AM191" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AN191" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AO191" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AP191" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AQ191" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AR191" s="89" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AS191" s="89" t="s">
         <v>35</v>
@@ -21409,7 +21415,7 @@
     </row>
     <row r="195" spans="1:55" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="47" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B195" s="39"/>
       <c r="C195" s="40"/>
@@ -21462,7 +21468,7 @@
     </row>
     <row r="196" spans="1:55" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="60" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B196" s="25" t="s">
         <v>16</v>
@@ -21912,37 +21918,37 @@
         <v>36</v>
       </c>
       <c r="AS199" s="41" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AT199" s="41" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU199" s="89" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AV199" s="89" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AW199" s="89" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="AX199" s="89" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AY199" s="89" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AZ199" s="89" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BA199" s="89" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BB199" s="89" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="BC199" s="89" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="200" spans="1:55" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -22225,7 +22231,7 @@
     </row>
     <row r="203" spans="1:55" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="60" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B203" s="39"/>
       <c r="C203" s="40"/>
@@ -22646,37 +22652,37 @@
         <v>36</v>
       </c>
       <c r="AS206" s="41" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AT206" s="41" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AU206" s="41" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AV206" s="41" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AW206" s="41" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AX206" s="41" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AY206" s="41" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AZ206" s="41" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="BA206" s="41" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="BB206" s="41" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="BC206" s="41" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="207" spans="1:55" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -23377,7 +23383,7 @@
         <v>10</v>
       </c>
       <c r="AS213" s="89" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="AT213" s="55">
         <v>10</v>
@@ -23925,7 +23931,7 @@
         <v>9.5</v>
       </c>
       <c r="BC218" s="55" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="219" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -24367,49 +24373,49 @@
         <v>80</v>
       </c>
       <c r="AD223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AE223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AF223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AG223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AH223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AI223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AJ223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AK223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AL223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AM223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AN223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AO223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AP223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AQ223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AR223" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AS223" s="89" t="s">
         <v>36</v>
@@ -24712,7 +24718,7 @@
     </row>
     <row r="227" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A227" s="47" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B227" s="25"/>
       <c r="C227" s="25"/>
@@ -24765,7 +24771,7 @@
     </row>
     <row r="228" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A228" s="60" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B228" s="25"/>
       <c r="C228" s="25"/>
@@ -24884,58 +24890,58 @@
       <c r="Y229" s="41"/>
       <c r="Z229" s="41"/>
       <c r="AA229" s="114" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="AB229" s="114" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="AC229" s="114" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="AD229" s="114" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="AE229" s="114" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="AF229" s="114" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AG229" s="114" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AH229" s="114" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AI229" s="114" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AJ229" s="114" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AK229" s="114" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AL229" s="114" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AM229" s="114" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AN229" s="54" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AO229" s="114" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AP229" s="114" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AQ229" s="114" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AR229" s="114" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AS229" s="113">
         <v>13</v>
@@ -25099,91 +25105,91 @@
       <c r="Y231" s="41"/>
       <c r="Z231" s="41"/>
       <c r="AA231" s="113" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="AB231" s="113" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="AC231" s="113" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="AD231" s="113" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="AE231" s="113" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="AF231" s="113" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="AG231" s="113" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="AH231" s="113" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="AI231" s="113" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="AJ231" s="113" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="AK231" s="113" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="AL231" s="113" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="AM231" s="113" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="AN231" s="113" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="AO231" s="113" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="AP231" s="113" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="AQ231" s="113" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="AR231" s="113" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="AS231" s="113" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="AT231" s="113" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="AU231" s="113" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="AV231" s="113" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="AW231" s="113" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="AX231" s="113" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="AY231" s="113" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="AZ231" s="113" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="BA231" s="113" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="BB231" s="113" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="BC231" s="113" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="232" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -25250,7 +25256,7 @@
     </row>
     <row r="233" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A233" s="60" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B233" s="25"/>
       <c r="C233" s="25"/>
@@ -25581,91 +25587,91 @@
       <c r="Y236" s="41"/>
       <c r="Z236" s="41"/>
       <c r="AA236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AB236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AC236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AD236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AE236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AF236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AG236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AH236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AI236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AJ236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AK236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AL236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AM236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AN236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AO236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AP236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AQ236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AR236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AS236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AT236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AU236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AV236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AW236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AX236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AY236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AZ236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="BA236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="BB236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="BC236" s="113" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="237" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -26028,85 +26034,85 @@
         <v>16</v>
       </c>
       <c r="D241" s="52" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E241" s="52" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F241" s="52" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G241" s="52" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="H241" s="52" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="I241" s="52" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="J241" s="52" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="K241" s="52" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="L241" s="52" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="M241" s="52" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="N241" s="52" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="O241" s="52" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="P241" s="52" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="Q241" s="52" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="R241" s="52" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="S241" s="52" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="T241" s="52" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="U241" s="52" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="V241" s="52" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="W241" s="52" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="X241" s="52" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="Y241" s="52" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="Z241" s="52" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AA241" s="14">
         <v>18</v>
       </c>
       <c r="AB241" s="52" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AC241" s="52" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AD241" s="52" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AE241" s="52" t="s">
         <v>24</v>
@@ -26640,79 +26646,79 @@
         <v>2</v>
       </c>
       <c r="AE246" s="52" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="AF246" s="52" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="AG246" s="52" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="AH246" s="52" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="AI246" s="52" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="AJ246" s="52" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AK246" s="52" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AL246" s="52" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AM246" s="52" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AN246" s="52" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AO246" s="52" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AP246" s="52" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AQ246" s="52" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AR246" s="52" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AS246" s="52" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="AT246" s="52" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="AU246" s="52" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="AV246" s="52" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="AW246" s="52" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="AX246" s="52" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="AY246" s="52" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="AZ246" s="52" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="BA246" s="52" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="BB246" s="52" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="BC246" s="52" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="247" spans="1:55" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -27138,25 +27144,25 @@
         <v>16</v>
       </c>
       <c r="U251" s="52" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="V251" s="52" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="W251" s="52" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="X251" s="52" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="Y251" s="52" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="Z251" s="52" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="AA251" s="52" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="AB251" s="52" t="s">
         <v>23</v>
@@ -27349,7 +27355,7 @@
         <v>20</v>
       </c>
       <c r="AA253" s="52" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="AB253" s="21">
         <v>23</v>
@@ -27361,22 +27367,22 @@
         <v>23</v>
       </c>
       <c r="AE253" s="52" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="AF253" s="52" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="AG253" s="52" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="AH253" s="52" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="AI253" s="52" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="AJ253" s="52" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="AK253" s="25" t="s">
         <v>16</v>
@@ -27843,10 +27849,10 @@
         <v>0</v>
       </c>
       <c r="AD258" s="93" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="AE258" s="93" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="AF258" s="93" t="s">
         <v>25</v>
@@ -28188,14 +28194,14 @@
       <c r="BC261" s="120"/>
     </row>
     <row r="262" spans="1:55" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A262" s="124" t="s">
-        <v>215</v>
-      </c>
-      <c r="B262" s="124"/>
-      <c r="C262" s="124"/>
-      <c r="D262" s="124"/>
-      <c r="E262" s="124"/>
-      <c r="F262" s="124"/>
+      <c r="A262" s="123" t="s">
+        <v>219</v>
+      </c>
+      <c r="B262" s="123"/>
+      <c r="C262" s="123"/>
+      <c r="D262" s="123"/>
+      <c r="E262" s="123"/>
+      <c r="F262" s="123"/>
       <c r="G262" s="26"/>
       <c r="H262" s="26"/>
       <c r="I262" s="26"/>
@@ -28347,7 +28353,7 @@
     </row>
     <row r="265" spans="1:55" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="125" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B265" s="125"/>
       <c r="C265" s="125"/>
@@ -28398,7 +28404,7 @@
     </row>
     <row r="266" spans="1:55" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="125" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B266" s="125"/>
       <c r="C266" s="125"/>
@@ -28448,32 +28454,32 @@
       <c r="AU266" s="125"/>
     </row>
     <row r="267" spans="1:55" s="2" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A267" s="123" t="s">
-        <v>182</v>
-      </c>
-      <c r="B267" s="123"/>
-      <c r="C267" s="123"/>
-      <c r="D267" s="123"/>
-      <c r="E267" s="123"/>
-      <c r="F267" s="123"/>
-      <c r="G267" s="123"/>
-      <c r="H267" s="123"/>
-      <c r="I267" s="123"/>
-      <c r="J267" s="123"/>
-      <c r="K267" s="123"/>
-      <c r="L267" s="123"/>
-      <c r="M267" s="123"/>
-      <c r="N267" s="123"/>
-      <c r="O267" s="123"/>
-      <c r="P267" s="123"/>
-      <c r="Q267" s="123"/>
-      <c r="R267" s="123"/>
-      <c r="S267" s="123"/>
-      <c r="T267" s="123"/>
-      <c r="U267" s="123"/>
-      <c r="V267" s="123"/>
-      <c r="W267" s="123"/>
-      <c r="X267" s="123"/>
+      <c r="A267" s="122" t="s">
+        <v>185</v>
+      </c>
+      <c r="B267" s="122"/>
+      <c r="C267" s="122"/>
+      <c r="D267" s="122"/>
+      <c r="E267" s="122"/>
+      <c r="F267" s="122"/>
+      <c r="G267" s="122"/>
+      <c r="H267" s="122"/>
+      <c r="I267" s="122"/>
+      <c r="J267" s="122"/>
+      <c r="K267" s="122"/>
+      <c r="L267" s="122"/>
+      <c r="M267" s="122"/>
+      <c r="N267" s="122"/>
+      <c r="O267" s="122"/>
+      <c r="P267" s="122"/>
+      <c r="Q267" s="122"/>
+      <c r="R267" s="122"/>
+      <c r="S267" s="122"/>
+      <c r="T267" s="122"/>
+      <c r="U267" s="122"/>
+      <c r="V267" s="122"/>
+      <c r="W267" s="122"/>
+      <c r="X267" s="122"/>
       <c r="Y267" s="119"/>
       <c r="Z267" s="119"/>
       <c r="AA267" s="119"/>
@@ -28550,32 +28556,32 @@
       <c r="AU268" s="118"/>
     </row>
     <row r="269" spans="1:55" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A269" s="122" t="s">
-        <v>185</v>
-      </c>
-      <c r="B269" s="122"/>
-      <c r="C269" s="122"/>
-      <c r="D269" s="122"/>
-      <c r="E269" s="122"/>
-      <c r="F269" s="122"/>
-      <c r="G269" s="122"/>
-      <c r="H269" s="122"/>
-      <c r="I269" s="122"/>
-      <c r="J269" s="122"/>
-      <c r="K269" s="122"/>
-      <c r="L269" s="122"/>
-      <c r="M269" s="122"/>
-      <c r="N269" s="122"/>
-      <c r="O269" s="122"/>
-      <c r="P269" s="122"/>
-      <c r="Q269" s="122"/>
-      <c r="R269" s="122"/>
-      <c r="S269" s="122"/>
-      <c r="T269" s="122"/>
-      <c r="U269" s="122"/>
-      <c r="V269" s="122"/>
-      <c r="W269" s="122"/>
-      <c r="X269" s="122"/>
+      <c r="A269" s="121" t="s">
+        <v>188</v>
+      </c>
+      <c r="B269" s="121"/>
+      <c r="C269" s="121"/>
+      <c r="D269" s="121"/>
+      <c r="E269" s="121"/>
+      <c r="F269" s="121"/>
+      <c r="G269" s="121"/>
+      <c r="H269" s="121"/>
+      <c r="I269" s="121"/>
+      <c r="J269" s="121"/>
+      <c r="K269" s="121"/>
+      <c r="L269" s="121"/>
+      <c r="M269" s="121"/>
+      <c r="N269" s="121"/>
+      <c r="O269" s="121"/>
+      <c r="P269" s="121"/>
+      <c r="Q269" s="121"/>
+      <c r="R269" s="121"/>
+      <c r="S269" s="121"/>
+      <c r="T269" s="121"/>
+      <c r="U269" s="121"/>
+      <c r="V269" s="121"/>
+      <c r="W269" s="121"/>
+      <c r="X269" s="121"/>
       <c r="Y269" s="31"/>
       <c r="Z269" s="31"/>
       <c r="AA269" s="31"/>
@@ -28602,7 +28608,7 @@
     </row>
     <row r="270" spans="1:55" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="38" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B270" s="38"/>
       <c r="C270" s="31"/>
@@ -28704,7 +28710,7 @@
     </row>
     <row r="272" spans="1:55" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="38" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B272" s="38"/>
       <c r="C272" s="31"/>
@@ -28947,7 +28953,7 @@
     </row>
     <row r="277" spans="1:47" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="68" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B277" s="66"/>
       <c r="C277" s="67"/>
@@ -28998,24 +29004,24 @@
     </row>
     <row r="278" spans="1:47" s="2" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="126" t="s">
-        <v>226</v>
-      </c>
-      <c r="B278" s="122"/>
-      <c r="C278" s="122"/>
-      <c r="D278" s="122"/>
-      <c r="E278" s="122"/>
-      <c r="F278" s="122"/>
-      <c r="G278" s="122"/>
-      <c r="H278" s="122"/>
-      <c r="I278" s="122"/>
-      <c r="J278" s="122"/>
-      <c r="K278" s="122"/>
-      <c r="L278" s="122"/>
-      <c r="M278" s="122"/>
-      <c r="N278" s="122"/>
-      <c r="O278" s="122"/>
-      <c r="P278" s="122"/>
-      <c r="Q278" s="122"/>
+        <v>230</v>
+      </c>
+      <c r="B278" s="121"/>
+      <c r="C278" s="121"/>
+      <c r="D278" s="121"/>
+      <c r="E278" s="121"/>
+      <c r="F278" s="121"/>
+      <c r="G278" s="121"/>
+      <c r="H278" s="121"/>
+      <c r="I278" s="121"/>
+      <c r="J278" s="121"/>
+      <c r="K278" s="121"/>
+      <c r="L278" s="121"/>
+      <c r="M278" s="121"/>
+      <c r="N278" s="121"/>
+      <c r="O278" s="121"/>
+      <c r="P278" s="121"/>
+      <c r="Q278" s="121"/>
       <c r="R278" s="66"/>
       <c r="S278" s="66"/>
       <c r="T278" s="66"/>
@@ -29049,7 +29055,7 @@
     </row>
     <row r="279" spans="1:47" s="90" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="126" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B279" s="126"/>
       <c r="C279" s="126"/>
@@ -29099,25 +29105,25 @@
       <c r="AU279" s="117"/>
     </row>
     <row r="280" spans="1:47" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A280" s="122" t="s">
-        <v>138</v>
-      </c>
-      <c r="B280" s="122"/>
-      <c r="C280" s="122"/>
-      <c r="D280" s="122"/>
-      <c r="E280" s="122"/>
-      <c r="F280" s="122"/>
-      <c r="G280" s="122"/>
-      <c r="H280" s="122"/>
-      <c r="I280" s="122"/>
-      <c r="J280" s="122"/>
-      <c r="K280" s="122"/>
-      <c r="L280" s="122"/>
-      <c r="M280" s="122"/>
-      <c r="N280" s="122"/>
-      <c r="O280" s="122"/>
-      <c r="P280" s="122"/>
-      <c r="Q280" s="122"/>
+      <c r="A280" s="121" t="s">
+        <v>141</v>
+      </c>
+      <c r="B280" s="121"/>
+      <c r="C280" s="121"/>
+      <c r="D280" s="121"/>
+      <c r="E280" s="121"/>
+      <c r="F280" s="121"/>
+      <c r="G280" s="121"/>
+      <c r="H280" s="121"/>
+      <c r="I280" s="121"/>
+      <c r="J280" s="121"/>
+      <c r="K280" s="121"/>
+      <c r="L280" s="121"/>
+      <c r="M280" s="121"/>
+      <c r="N280" s="121"/>
+      <c r="O280" s="121"/>
+      <c r="P280" s="121"/>
+      <c r="Q280" s="121"/>
       <c r="R280" s="68"/>
       <c r="S280" s="68"/>
       <c r="T280" s="68"/>
@@ -29151,7 +29157,7 @@
     </row>
     <row r="281" spans="1:47" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" s="68" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B281" s="68"/>
       <c r="C281" s="68"/>
@@ -29216,11 +29222,11 @@
     <row r="283" spans="1:47" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B1:AU1"/>
     <mergeCell ref="A280:Q280"/>
     <mergeCell ref="A269:X269"/>
     <mergeCell ref="A267:X267"/>
     <mergeCell ref="A262:F262"/>
+    <mergeCell ref="B1:AU1"/>
     <mergeCell ref="A265:AU265"/>
     <mergeCell ref="A266:AU266"/>
     <mergeCell ref="A278:Q278"/>

</xml_diff>